<commit_message>
adicionado coluna apenas para data
</commit_message>
<xml_diff>
--- a/sobs - template.xlsx
+++ b/sobs - template.xlsx
@@ -2,29 +2,30 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Planejamento SG\Documents\Projetos Trabalho\Programa SOB (Execução)\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="669"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="669" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="sob11 (6)" sheetId="34" r:id="rId1"/>
-    <sheet name="sob11 (5)" sheetId="33" r:id="rId2"/>
-    <sheet name="sob11 (4)" sheetId="32" r:id="rId3"/>
-    <sheet name="sob11 (3)" sheetId="31" r:id="rId4"/>
-    <sheet name="sob11 (2)" sheetId="30" r:id="rId5"/>
-    <sheet name="sob11" sheetId="24" r:id="rId6"/>
+    <sheet name="1" sheetId="34" r:id="rId1"/>
+    <sheet name="2" sheetId="33" r:id="rId2"/>
+    <sheet name="3" sheetId="32" r:id="rId3"/>
+    <sheet name="4" sheetId="31" r:id="rId4"/>
+    <sheet name="5" sheetId="30" r:id="rId5"/>
+    <sheet name="6" sheetId="24" r:id="rId6"/>
+    <sheet name="7" sheetId="35" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
   <si>
     <t>COMP12</t>
   </si>
@@ -32,43 +33,52 @@
     <t>A3279</t>
   </si>
   <si>
-    <t>081120170900</t>
-  </si>
-  <si>
-    <t>081120170905</t>
-  </si>
-  <si>
-    <t>081120170906</t>
-  </si>
-  <si>
-    <t>081120170911</t>
-  </si>
-  <si>
-    <t>081120170912</t>
-  </si>
-  <si>
-    <t>081120170917</t>
-  </si>
-  <si>
-    <t>081120170918</t>
-  </si>
-  <si>
-    <t>081120170923</t>
-  </si>
-  <si>
-    <t>081120170924</t>
-  </si>
-  <si>
-    <t>081120170929</t>
-  </si>
-  <si>
-    <t>081120170930</t>
-  </si>
-  <si>
-    <t>081120170935</t>
-  </si>
-  <si>
-    <t>07/11/2017</t>
+    <t>0120180600</t>
+  </si>
+  <si>
+    <t>0120180605</t>
+  </si>
+  <si>
+    <t>0120180606</t>
+  </si>
+  <si>
+    <t>0120180611</t>
+  </si>
+  <si>
+    <t>0120180612</t>
+  </si>
+  <si>
+    <t>0120180617</t>
+  </si>
+  <si>
+    <t>0120180618</t>
+  </si>
+  <si>
+    <t>0120180623</t>
+  </si>
+  <si>
+    <t>0120180624</t>
+  </si>
+  <si>
+    <t>0120180629</t>
+  </si>
+  <si>
+    <t>0120180630</t>
+  </si>
+  <si>
+    <t>0120180635</t>
+  </si>
+  <si>
+    <t>0120180636</t>
+  </si>
+  <si>
+    <t>0120180641</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>02/01/2018</t>
   </si>
 </sst>
 </file>
@@ -414,37 +424,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <sheetPr codeName="Planilha1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="14" style="1"/>
+    <col min="4" max="5" width="14" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -453,40 +468,43 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <sheetPr codeName="Planilha2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="14" style="1"/>
+    <col min="4" max="5" width="14" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -495,39 +513,42 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <sheetPr codeName="Planilha3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="14" style="1"/>
+    <col min="4" max="5" width="14" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -536,39 +557,42 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <sheetPr codeName="Planilha4"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="14" style="1"/>
+    <col min="4" max="5" width="14" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -577,39 +601,42 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <sheetPr codeName="Planilha5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="14" style="1"/>
+    <col min="4" max="5" width="14" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -618,39 +645,86 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <sheetPr codeName="Planilha6"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="14" style="1"/>
+    <col min="4" max="5" width="14" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Planilha7"/>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="5" width="14" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>